<commit_message>
updated logic for step defs
</commit_message>
<xml_diff>
--- a/lib/testData/CloudAutomation_TestData.xlsx
+++ b/lib/testData/CloudAutomation_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venkat\IntellijProjects\SeleniumFSCM\lib\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venkat\IntellijProjects\SeleniumFSCM\lib\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE46F87-A364-4B9B-BA26-1B6A6CA06DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF295E5E-4B01-447D-9E2C-DD5285DD972D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F306060A-5D11-4DCC-9369-A4EAEF2038D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16776" xr2:uid="{F306060A-5D11-4DCC-9369-A4EAEF2038D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Username</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Approver</t>
   </si>
   <si>
-    <t>Mercury</t>
-  </si>
-  <si>
     <t>Username2</t>
   </si>
   <si>
@@ -92,13 +89,57 @@
   </si>
   <si>
     <t>journal_line2_desc</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Spreadsheet</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>1111.1123.1234</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>2222.1123.1234</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>Successful login with valid credentials</t>
+  </si>
+  <si>
+    <t>Unsuccessful login with invalid credentials</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABC0876-8DE7-42EA-8737-6EBE3ED19ACE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>0</v>
@@ -470,13 +512,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -484,10 +526,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>4</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -497,72 +539,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50716B26-2368-4292-936C-570601C8E283}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.109375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.88671875"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="17.21875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.33203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.21875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.21875"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.44140625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="20.21875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.5546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.88671875"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="17.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.21875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.21875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.44140625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.21875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="G1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="H1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="I1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="J1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="K1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="L1" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="N1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="L1" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="N1" t="s" s="0">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45925</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I2" s="0">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K2" s="0">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="N2" s="0">
+        <v>120</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45925</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I3" s="0">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K3" s="0">
+        <v>120</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="N3" s="0">
+        <v>120</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>